<commit_message>
Add US big (0.43/0.42) coefficients to everything
</commit_message>
<xml_diff>
--- a/output/lnUSDummyModelTripleInteractionlnMortSq2.xlsx
+++ b/output/lnUSDummyModelTripleInteractionlnMortSq2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bz22\Desktop\ComparativeMortality\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFABAAE-9D78-4223-B9E5-74F8558E000E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA21F60-E2A9-4C01-AD3F-C8CB64E4E9CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lnUSDummyModelTripleInteraction" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="249">
   <si>
     <t>AllCountries</t>
   </si>
@@ -768,6 +768,9 @@
   </si>
   <si>
     <t>Add Coef</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -3176,22 +3179,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-9.5576900000000006E-2</c:v>
+                  <c:v>0.33623239999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.1443758</c:v>
+                  <c:v>0.28743350000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.1280452</c:v>
+                  <c:v>0.30376409999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-2.3748700000000001E-2</c:v>
+                  <c:v>0.4080606</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-2.5717400000000001E-2</c:v>
+                  <c:v>0.40609190000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.5763800000000002E-2</c:v>
+                  <c:v>0.48757309999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3263,22 +3266,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-0.20451009999999997</c:v>
+                  <c:v>0.22729920000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.15122239999999998</c:v>
+                  <c:v>0.28058689999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.19988719999999999</c:v>
+                  <c:v>0.23192210000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.1955712</c:v>
+                  <c:v>0.23623810000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-7.8326699999999985E-2</c:v>
+                  <c:v>0.35348259999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.187247</c:v>
+                  <c:v>0.6190563</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3350,22 +3353,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-0.2247189</c:v>
+                  <c:v>0.20709040000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.32084370000000001</c:v>
+                  <c:v>0.1109656</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.37554529999999997</c:v>
+                  <c:v>5.6263999999999981E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.28083330000000001</c:v>
+                  <c:v>0.150976</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.2139875</c:v>
+                  <c:v>0.21782180000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-3.8567699999999996E-2</c:v>
+                  <c:v>0.39324160000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3437,22 +3440,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-0.24398829999999999</c:v>
+                  <c:v>0.18782100000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.40028639999999999</c:v>
+                  <c:v>3.152290000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.45993079999999997</c:v>
+                  <c:v>-2.8121499999999966E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.38585030000000003</c:v>
+                  <c:v>4.5959000000000028E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.32111109999999998</c:v>
+                  <c:v>0.11069820000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.2282469</c:v>
+                  <c:v>0.2035624</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3524,22 +3527,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-0.42010260000000005</c:v>
+                  <c:v>1.1706700000000014E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.50712279999999998</c:v>
+                  <c:v>-7.5313499999999978E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.48603459999999998</c:v>
+                  <c:v>-5.4225299999999976E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.4040434</c:v>
+                  <c:v>2.776590000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.39425060000000001</c:v>
+                  <c:v>3.75587E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.33999800000000002</c:v>
+                  <c:v>9.1811299999999985E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3611,22 +3614,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-0.55440870000000009</c:v>
+                  <c:v>-0.12259939999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.59397469999999997</c:v>
+                  <c:v>-0.16216539999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.52585350000000008</c:v>
+                  <c:v>-9.4044199999999967E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.46110810000000008</c:v>
+                  <c:v>-2.9298800000000014E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.42330570000000006</c:v>
+                  <c:v>8.5036E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.42371170000000002</c:v>
+                  <c:v>8.0975999999999826E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3700,22 +3703,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-0.63400629999999991</c:v>
+                  <c:v>-0.20219700000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.66070269999999987</c:v>
+                  <c:v>-0.22889339999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.59403199999999989</c:v>
+                  <c:v>-0.1622227</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.56341069999999993</c:v>
+                  <c:v>-0.13160140000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.51994109999999993</c:v>
+                  <c:v>-8.8131800000000038E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.51149899999999993</c:v>
+                  <c:v>-7.968970000000003E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3789,22 +3792,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-0.56177909999999998</c:v>
+                  <c:v>-0.12996979999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.62453150000000002</c:v>
+                  <c:v>-0.19272220000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.61896510000000005</c:v>
+                  <c:v>-0.18715580000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.56395919999999999</c:v>
+                  <c:v>-0.13214989999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.54239300000000001</c:v>
+                  <c:v>-0.11058370000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.56449490000000002</c:v>
+                  <c:v>-0.13268560000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4133,28 +4136,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-9.5576900000000006E-2</c:v>
+                  <c:v>0.33623239999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.20451009999999997</c:v>
+                  <c:v>0.22729920000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.2247189</c:v>
+                  <c:v>0.20709040000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.24398829999999999</c:v>
+                  <c:v>0.18782100000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.42010260000000005</c:v>
+                  <c:v>1.1706700000000014E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.55440870000000009</c:v>
+                  <c:v>-0.12259939999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.63400629999999991</c:v>
+                  <c:v>-0.20219700000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.56177909999999998</c:v>
+                  <c:v>-0.12996979999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4231,28 +4234,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-0.1443758</c:v>
+                  <c:v>0.28743350000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.15122239999999998</c:v>
+                  <c:v>0.28058689999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.32084370000000001</c:v>
+                  <c:v>0.1109656</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.40028639999999999</c:v>
+                  <c:v>3.152290000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.50712279999999998</c:v>
+                  <c:v>-7.5313499999999978E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.59397469999999997</c:v>
+                  <c:v>-0.16216539999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.66070269999999987</c:v>
+                  <c:v>-0.22889339999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.62453150000000002</c:v>
+                  <c:v>-0.19272220000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4329,28 +4332,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-0.1280452</c:v>
+                  <c:v>0.30376409999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.19988719999999999</c:v>
+                  <c:v>0.23192210000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.37554529999999997</c:v>
+                  <c:v>5.6263999999999981E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.45993079999999997</c:v>
+                  <c:v>-2.8121499999999966E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.48603459999999998</c:v>
+                  <c:v>-5.4225299999999976E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.52585350000000008</c:v>
+                  <c:v>-9.4044199999999967E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.59403199999999989</c:v>
+                  <c:v>-0.1622227</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.61896510000000005</c:v>
+                  <c:v>-0.18715580000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4427,28 +4430,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-2.3748700000000001E-2</c:v>
+                  <c:v>0.4080606</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.1955712</c:v>
+                  <c:v>0.23623810000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.28083330000000001</c:v>
+                  <c:v>0.150976</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.38585030000000003</c:v>
+                  <c:v>4.5959000000000028E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.4040434</c:v>
+                  <c:v>2.776590000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.46110810000000008</c:v>
+                  <c:v>-2.9298800000000014E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.56341069999999993</c:v>
+                  <c:v>-0.13160140000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.56395919999999999</c:v>
+                  <c:v>-0.13214989999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4525,28 +4528,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-2.5717400000000001E-2</c:v>
+                  <c:v>0.40609190000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-7.8326699999999985E-2</c:v>
+                  <c:v>0.35348259999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.2139875</c:v>
+                  <c:v>0.21782180000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.32111109999999998</c:v>
+                  <c:v>0.11069820000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.39425060000000001</c:v>
+                  <c:v>3.75587E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.42330570000000006</c:v>
+                  <c:v>8.5036E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.51994109999999993</c:v>
+                  <c:v>-8.8131800000000038E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.54239300000000001</c:v>
+                  <c:v>-0.11058370000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4623,28 +4626,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>5.5763800000000002E-2</c:v>
+                  <c:v>0.48757309999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.187247</c:v>
+                  <c:v>0.6190563</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3.8567699999999996E-2</c:v>
+                  <c:v>0.39324160000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.2282469</c:v>
+                  <c:v>0.2035624</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.33999800000000002</c:v>
+                  <c:v>9.1811299999999985E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.42371170000000002</c:v>
+                  <c:v>8.0975999999999826E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.51149899999999993</c:v>
+                  <c:v>-7.968970000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.56449490000000002</c:v>
+                  <c:v>-0.13268560000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6685,22 +6688,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-8.2736199999999996E-2</c:v>
+                  <c:v>0.34453690000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.1238089</c:v>
+                  <c:v>0.30346420000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.10956299999999999</c:v>
+                  <c:v>0.3177101</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.44046E-2</c:v>
+                  <c:v>0.41286850000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.0864900000000001E-2</c:v>
+                  <c:v>0.39640819999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.1643799999999999E-2</c:v>
+                  <c:v>0.48891689999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6772,22 +6775,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-0.19365070000000001</c:v>
+                  <c:v>0.23362240000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.13369059999999999</c:v>
+                  <c:v>0.29358250000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.18387580000000001</c:v>
+                  <c:v>0.24339730000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.18968409999999999</c:v>
+                  <c:v>0.23758900000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-8.4181500000000006E-2</c:v>
+                  <c:v>0.3430916</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.1710189</c:v>
+                  <c:v>0.59829200000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6859,22 +6862,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-0.21749609999999997</c:v>
+                  <c:v>0.20977700000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.30781799999999998</c:v>
+                  <c:v>0.11945510000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.362456</c:v>
+                  <c:v>6.4817100000000016E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.27196239999999999</c:v>
+                  <c:v>0.15531070000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.20224349999999999</c:v>
+                  <c:v>0.22502960000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2.0099500000000006E-2</c:v>
+                  <c:v>0.40717360000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6946,22 +6949,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-0.23572369999999998</c:v>
+                  <c:v>0.19154940000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.38977989999999996</c:v>
+                  <c:v>3.7493200000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.45770499999999992</c:v>
+                  <c:v>-3.0431899999999956E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.37527060000000001</c:v>
+                  <c:v>5.2002500000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.29594489999999996</c:v>
+                  <c:v>0.13132820000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.2021086</c:v>
+                  <c:v>0.22516450000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7033,22 +7036,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-0.41074839999999996</c:v>
+                  <c:v>1.6524700000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.49898370000000003</c:v>
+                  <c:v>-7.1710599999999958E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.49047819999999998</c:v>
+                  <c:v>-6.3205099999999959E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.40029139999999996</c:v>
+                  <c:v>2.6981699999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.38855119999999999</c:v>
+                  <c:v>3.8721900000000031E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.32179610000000003</c:v>
+                  <c:v>0.10547700000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7120,22 +7123,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-0.54465839999999999</c:v>
+                  <c:v>-0.11738529999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.5843453999999999</c:v>
+                  <c:v>-0.1570723</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.52644659999999999</c:v>
+                  <c:v>-9.917349999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.45588609999999996</c:v>
+                  <c:v>-2.8613E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.4227593999999999</c:v>
+                  <c:v>4.5137000000000094E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.409551</c:v>
+                  <c:v>1.7722100000000018E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7209,22 +7212,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-0.62729639999999998</c:v>
+                  <c:v>-0.20002329999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.65378219999999998</c:v>
+                  <c:v>-0.22650909999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.60023779999999993</c:v>
+                  <c:v>-0.17296470000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.5664518999999999</c:v>
+                  <c:v>-0.13917879999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.52368949999999992</c:v>
+                  <c:v>-9.6416400000000013E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.50304589999999993</c:v>
+                  <c:v>-7.5772800000000029E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7298,22 +7301,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-0.55715610000000004</c:v>
+                  <c:v>-0.12988300000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.61997610000000003</c:v>
+                  <c:v>-0.19270300000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.6310135</c:v>
+                  <c:v>-0.20374039999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.57389100000000004</c:v>
+                  <c:v>-0.14661790000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.55308420000000003</c:v>
+                  <c:v>-0.12581110000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.56193879999999996</c:v>
+                  <c:v>-0.13466569999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7642,28 +7645,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-8.2736199999999996E-2</c:v>
+                  <c:v>0.34453690000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.19365070000000001</c:v>
+                  <c:v>0.23362240000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.21749609999999997</c:v>
+                  <c:v>0.20977700000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.23572369999999998</c:v>
+                  <c:v>0.19154940000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.41074839999999996</c:v>
+                  <c:v>1.6524700000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.54465839999999999</c:v>
+                  <c:v>-0.11738529999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.62729639999999998</c:v>
+                  <c:v>-0.20002329999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.55715610000000004</c:v>
+                  <c:v>-0.12988300000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7740,28 +7743,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-0.1238089</c:v>
+                  <c:v>0.30346420000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.13369059999999999</c:v>
+                  <c:v>0.29358250000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.30781799999999998</c:v>
+                  <c:v>0.11945510000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.38977989999999996</c:v>
+                  <c:v>3.7493200000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.49898370000000003</c:v>
+                  <c:v>-7.1710599999999958E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.5843453999999999</c:v>
+                  <c:v>-0.1570723</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.65378219999999998</c:v>
+                  <c:v>-0.22650909999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.61997610000000003</c:v>
+                  <c:v>-0.19270300000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7838,28 +7841,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-0.10956299999999999</c:v>
+                  <c:v>0.3177101</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.18387580000000001</c:v>
+                  <c:v>0.24339730000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.362456</c:v>
+                  <c:v>6.4817100000000016E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.45770499999999992</c:v>
+                  <c:v>-3.0431899999999956E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.49047819999999998</c:v>
+                  <c:v>-6.3205099999999959E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.52644659999999999</c:v>
+                  <c:v>-9.917349999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.60023779999999993</c:v>
+                  <c:v>-0.17296470000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.6310135</c:v>
+                  <c:v>-0.20374039999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7936,28 +7939,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-1.44046E-2</c:v>
+                  <c:v>0.41286850000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.18968409999999999</c:v>
+                  <c:v>0.23758900000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.27196239999999999</c:v>
+                  <c:v>0.15531070000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.37527060000000001</c:v>
+                  <c:v>5.2002500000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.40029139999999996</c:v>
+                  <c:v>2.6981699999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.45588609999999996</c:v>
+                  <c:v>-2.8613E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.5664518999999999</c:v>
+                  <c:v>-0.13917879999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.57389100000000004</c:v>
+                  <c:v>-0.14661790000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8034,28 +8037,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-3.0864900000000001E-2</c:v>
+                  <c:v>0.39640819999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-8.4181500000000006E-2</c:v>
+                  <c:v>0.3430916</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.20224349999999999</c:v>
+                  <c:v>0.22502960000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.29594489999999996</c:v>
+                  <c:v>0.13132820000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.38855119999999999</c:v>
+                  <c:v>3.8721900000000031E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.4227593999999999</c:v>
+                  <c:v>4.5137000000000094E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.52368949999999992</c:v>
+                  <c:v>-9.6416400000000013E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.55308420000000003</c:v>
+                  <c:v>-0.12581110000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8132,28 +8135,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6.1643799999999999E-2</c:v>
+                  <c:v>0.48891689999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1710189</c:v>
+                  <c:v>0.59829200000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.0099500000000006E-2</c:v>
+                  <c:v>0.40717360000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.2021086</c:v>
+                  <c:v>0.22516450000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.32179610000000003</c:v>
+                  <c:v>0.10547700000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.409551</c:v>
+                  <c:v>1.7722100000000018E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.50304589999999993</c:v>
+                  <c:v>-7.5772800000000029E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.56193879999999996</c:v>
+                  <c:v>-0.13466569999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12932,15 +12935,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>347662</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2043112</xdr:colOff>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>42861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -13051,15 +13054,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>403412</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>78441</xdr:rowOff>
+      <xdr:colOff>638735</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>33617</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>246529</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>179295</xdr:rowOff>
+      <xdr:colOff>481852</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13087,15 +13090,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>117659</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>90766</xdr:rowOff>
+      <xdr:colOff>431425</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>34737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>89646</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>156881</xdr:rowOff>
+      <xdr:colOff>403412</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>100852</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13422,8 +13425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C237"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62:C67"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16029,8 +16032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N37" sqref="N37"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17538,10 +17541,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6752113A-E80F-4D8E-962A-42C6198FCF3D}">
-  <dimension ref="A2:I23"/>
+  <dimension ref="A2:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:I19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17577,22 +17580,28 @@
         <v>237</v>
       </c>
       <c r="B3">
-        <v>-9.5576900000000006E-2</v>
+        <f>-0.0955769+$B$27</f>
+        <v>0.33623239999999999</v>
       </c>
       <c r="C3">
-        <v>-0.1443758</v>
+        <f>B27-0.1443758</f>
+        <v>0.28743350000000001</v>
       </c>
       <c r="D3">
-        <v>-0.1280452</v>
+        <f>B27-0.1280452</f>
+        <v>0.30376409999999998</v>
       </c>
       <c r="E3">
-        <v>-2.3748700000000001E-2</v>
+        <f>B27-0.0237487</f>
+        <v>0.4080606</v>
       </c>
       <c r="F3">
-        <v>-2.5717400000000001E-2</v>
+        <f>B27-0.0257174</f>
+        <v>0.40609190000000001</v>
       </c>
       <c r="G3">
-        <v>5.5763800000000002E-2</v>
+        <f>B27+0.0557638</f>
+        <v>0.48757309999999998</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -17600,22 +17609,28 @@
         <v>238</v>
       </c>
       <c r="B4">
-        <v>-0.20451009999999997</v>
+        <f>-0.2045101+B27</f>
+        <v>0.22729920000000001</v>
       </c>
       <c r="C4">
-        <v>-0.15122239999999998</v>
+        <f>B27-0.1512224</f>
+        <v>0.28058689999999997</v>
       </c>
       <c r="D4">
-        <v>-0.19988719999999999</v>
+        <f>B27-0.1998872</f>
+        <v>0.23192210000000002</v>
       </c>
       <c r="E4">
-        <v>-0.1955712</v>
+        <f>B27-0.1955712</f>
+        <v>0.23623810000000001</v>
       </c>
       <c r="F4">
-        <v>-7.8326699999999985E-2</v>
+        <f>B27-0.0783267</f>
+        <v>0.35348259999999998</v>
       </c>
       <c r="G4">
-        <v>0.187247</v>
+        <f>0.187247+B27</f>
+        <v>0.6190563</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -17623,22 +17638,28 @@
         <v>239</v>
       </c>
       <c r="B5">
-        <v>-0.2247189</v>
+        <f>-0.2247189+B27</f>
+        <v>0.20709040000000001</v>
       </c>
       <c r="C5">
-        <v>-0.32084370000000001</v>
+        <f>B27-0.3208437</f>
+        <v>0.1109656</v>
       </c>
       <c r="D5">
-        <v>-0.37554529999999997</v>
+        <f>B27-0.3755453</f>
+        <v>5.6263999999999981E-2</v>
       </c>
       <c r="E5">
-        <v>-0.28083330000000001</v>
+        <f>B27-0.2808333</f>
+        <v>0.150976</v>
       </c>
       <c r="F5">
-        <v>-0.2139875</v>
+        <f>B27-0.2139875</f>
+        <v>0.21782180000000001</v>
       </c>
       <c r="G5">
-        <v>-3.8567699999999996E-2</v>
+        <f>B27-0.0385677</f>
+        <v>0.39324160000000002</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -17646,22 +17667,28 @@
         <v>240</v>
       </c>
       <c r="B6">
-        <v>-0.24398829999999999</v>
+        <f>-0.2439883+B27</f>
+        <v>0.18782100000000002</v>
       </c>
       <c r="C6">
-        <v>-0.40028639999999999</v>
+        <f>B27-0.4002864</f>
+        <v>3.152290000000002E-2</v>
       </c>
       <c r="D6">
-        <v>-0.45993079999999997</v>
+        <f>B27-0.4599308</f>
+        <v>-2.8121499999999966E-2</v>
       </c>
       <c r="E6">
-        <v>-0.38585030000000003</v>
+        <f>B27-0.3858503</f>
+        <v>4.5959000000000028E-2</v>
       </c>
       <c r="F6">
-        <v>-0.32111109999999998</v>
+        <f>B27-0.3211111</f>
+        <v>0.11069820000000002</v>
       </c>
       <c r="G6">
-        <v>-0.2282469</v>
+        <f>B27-0.2282469</f>
+        <v>0.2035624</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -17669,22 +17696,28 @@
         <v>241</v>
       </c>
       <c r="B7">
-        <v>-0.42010260000000005</v>
+        <f>-0.4201026+B27</f>
+        <v>1.1706700000000014E-2</v>
       </c>
       <c r="C7">
-        <v>-0.50712279999999998</v>
+        <f>B27-0.5071228</f>
+        <v>-7.5313499999999978E-2</v>
       </c>
       <c r="D7">
-        <v>-0.48603459999999998</v>
+        <f>B27-0.4860346</f>
+        <v>-5.4225299999999976E-2</v>
       </c>
       <c r="E7">
-        <v>-0.4040434</v>
+        <f>B27-0.4040434</f>
+        <v>2.776590000000001E-2</v>
       </c>
       <c r="F7">
-        <v>-0.39425060000000001</v>
+        <f>B27-0.3942506</f>
+        <v>3.75587E-2</v>
       </c>
       <c r="G7">
-        <v>-0.33999800000000002</v>
+        <f>B27-0.339998</f>
+        <v>9.1811299999999985E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -17692,22 +17725,28 @@
         <v>242</v>
       </c>
       <c r="B8">
-        <v>-0.55440870000000009</v>
+        <f>-0.5544087+B27</f>
+        <v>-0.12259939999999997</v>
       </c>
       <c r="C8">
-        <v>-0.59397469999999997</v>
+        <f>B27-0.5939747</f>
+        <v>-0.16216539999999996</v>
       </c>
       <c r="D8">
-        <v>-0.52585350000000008</v>
+        <f>B27-0.5258535</f>
+        <v>-9.4044199999999967E-2</v>
       </c>
       <c r="E8">
-        <v>-0.46110810000000008</v>
+        <f>B27-0.4611081</f>
+        <v>-2.9298800000000014E-2</v>
       </c>
       <c r="F8">
-        <v>-0.42330570000000006</v>
+        <f>B27-0.4233057</f>
+        <v>8.5036E-3</v>
       </c>
       <c r="G8">
-        <v>-0.42371170000000002</v>
+        <f>B27-0.4237117</f>
+        <v>8.0975999999999826E-3</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -17715,22 +17754,28 @@
         <v>243</v>
       </c>
       <c r="B9">
-        <v>-0.63400629999999991</v>
+        <f>-0.6340063+B27</f>
+        <v>-0.20219700000000002</v>
       </c>
       <c r="C9">
-        <v>-0.66070269999999987</v>
+        <f>B27-0.6607027</f>
+        <v>-0.22889339999999997</v>
       </c>
       <c r="D9">
-        <v>-0.59403199999999989</v>
+        <f>B27-0.594032</f>
+        <v>-0.1622227</v>
       </c>
       <c r="E9">
-        <v>-0.56341069999999993</v>
+        <f>B27-0.5634107</f>
+        <v>-0.13160140000000004</v>
       </c>
       <c r="F9">
-        <v>-0.51994109999999993</v>
+        <f>B27-0.5199411</f>
+        <v>-8.8131800000000038E-2</v>
       </c>
       <c r="G9">
-        <v>-0.51149899999999993</v>
+        <f>B27-0.511499</f>
+        <v>-7.968970000000003E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -17738,22 +17783,28 @@
         <v>244</v>
       </c>
       <c r="B10">
-        <v>-0.56177909999999998</v>
+        <f>-0.5617791+B27</f>
+        <v>-0.12996979999999997</v>
       </c>
       <c r="C10">
-        <v>-0.62453150000000002</v>
+        <f>B27-0.6245315</f>
+        <v>-0.19272220000000001</v>
       </c>
       <c r="D10">
-        <v>-0.61896510000000005</v>
+        <f>B27-0.6189651</f>
+        <v>-0.18715580000000004</v>
       </c>
       <c r="E10">
-        <v>-0.56395919999999999</v>
+        <f>B27-0.5639592</f>
+        <v>-0.13214989999999999</v>
       </c>
       <c r="F10">
-        <v>-0.54239300000000001</v>
+        <f>B27-0.542393</f>
+        <v>-0.11058370000000001</v>
       </c>
       <c r="G10">
-        <v>-0.56449490000000002</v>
+        <f>B27-0.5644949</f>
+        <v>-0.13268560000000001</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -17798,28 +17849,36 @@
         <v>1960</v>
       </c>
       <c r="B18">
-        <v>-9.5576900000000006E-2</v>
+        <f>B27-0.0955769</f>
+        <v>0.33623239999999999</v>
       </c>
       <c r="C18">
-        <v>-0.20451009999999997</v>
+        <f>B27-0.2045101</f>
+        <v>0.22729920000000001</v>
       </c>
       <c r="D18">
-        <v>-0.2247189</v>
+        <f>B27-0.2247189</f>
+        <v>0.20709040000000001</v>
       </c>
       <c r="E18">
-        <v>-0.24398829999999999</v>
+        <f>B27-0.2439883</f>
+        <v>0.18782100000000002</v>
       </c>
       <c r="F18">
-        <v>-0.42010260000000005</v>
+        <f>B27-0.4201026</f>
+        <v>1.1706700000000014E-2</v>
       </c>
       <c r="G18">
-        <v>-0.55440870000000009</v>
+        <f>B27-0.5544087</f>
+        <v>-0.12259939999999997</v>
       </c>
       <c r="H18">
-        <v>-0.63400629999999991</v>
+        <f>B27-0.6340063</f>
+        <v>-0.20219700000000002</v>
       </c>
       <c r="I18">
-        <v>-0.56177909999999998</v>
+        <f>B27-0.5617791</f>
+        <v>-0.12996979999999997</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -17827,28 +17886,36 @@
         <v>1970</v>
       </c>
       <c r="B19">
-        <v>-0.1443758</v>
+        <f>B27-0.1443758</f>
+        <v>0.28743350000000001</v>
       </c>
       <c r="C19">
-        <v>-0.15122239999999998</v>
+        <f>B27-0.1512224</f>
+        <v>0.28058689999999997</v>
       </c>
       <c r="D19">
-        <v>-0.32084370000000001</v>
+        <f>B27-0.3208437</f>
+        <v>0.1109656</v>
       </c>
       <c r="E19">
-        <v>-0.40028639999999999</v>
+        <f>B27-0.4002864</f>
+        <v>3.152290000000002E-2</v>
       </c>
       <c r="F19">
-        <v>-0.50712279999999998</v>
+        <f>B27-0.5071228</f>
+        <v>-7.5313499999999978E-2</v>
       </c>
       <c r="G19">
-        <v>-0.59397469999999997</v>
+        <f>B27-0.5939747</f>
+        <v>-0.16216539999999996</v>
       </c>
       <c r="H19">
-        <v>-0.66070269999999987</v>
+        <f>B27-0.6607027</f>
+        <v>-0.22889339999999997</v>
       </c>
       <c r="I19">
-        <v>-0.62453150000000002</v>
+        <f>B27-0.6245315</f>
+        <v>-0.19272220000000001</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -17856,28 +17923,36 @@
         <v>1980</v>
       </c>
       <c r="B20">
-        <v>-0.1280452</v>
+        <f>B27-0.1280452</f>
+        <v>0.30376409999999998</v>
       </c>
       <c r="C20">
-        <v>-0.19988719999999999</v>
+        <f>B27-0.1998872</f>
+        <v>0.23192210000000002</v>
       </c>
       <c r="D20">
-        <v>-0.37554529999999997</v>
+        <f>B27-0.3755453</f>
+        <v>5.6263999999999981E-2</v>
       </c>
       <c r="E20">
-        <v>-0.45993079999999997</v>
+        <f>B27-0.4599308</f>
+        <v>-2.8121499999999966E-2</v>
       </c>
       <c r="F20">
-        <v>-0.48603459999999998</v>
+        <f>B27-0.4860346</f>
+        <v>-5.4225299999999976E-2</v>
       </c>
       <c r="G20">
-        <v>-0.52585350000000008</v>
+        <f>B27-0.5258535</f>
+        <v>-9.4044199999999967E-2</v>
       </c>
       <c r="H20">
-        <v>-0.59403199999999989</v>
+        <f>B27-0.594032</f>
+        <v>-0.1622227</v>
       </c>
       <c r="I20">
-        <v>-0.61896510000000005</v>
+        <f>B27-0.6189651</f>
+        <v>-0.18715580000000004</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -17885,28 +17960,36 @@
         <v>1990</v>
       </c>
       <c r="B21">
-        <v>-2.3748700000000001E-2</v>
+        <f>B27-0.0237487</f>
+        <v>0.4080606</v>
       </c>
       <c r="C21">
-        <v>-0.1955712</v>
+        <f>B27-0.1955712</f>
+        <v>0.23623810000000001</v>
       </c>
       <c r="D21">
-        <v>-0.28083330000000001</v>
+        <f>B27-0.2808333</f>
+        <v>0.150976</v>
       </c>
       <c r="E21">
-        <v>-0.38585030000000003</v>
+        <f>B27-0.3858503</f>
+        <v>4.5959000000000028E-2</v>
       </c>
       <c r="F21">
-        <v>-0.4040434</v>
+        <f>B27-0.4040434</f>
+        <v>2.776590000000001E-2</v>
       </c>
       <c r="G21">
-        <v>-0.46110810000000008</v>
+        <f>B27-0.4611081</f>
+        <v>-2.9298800000000014E-2</v>
       </c>
       <c r="H21">
-        <v>-0.56341069999999993</v>
+        <f>B27-0.5634107</f>
+        <v>-0.13160140000000004</v>
       </c>
       <c r="I21">
-        <v>-0.56395919999999999</v>
+        <f>B27-0.5639592</f>
+        <v>-0.13214989999999999</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -17914,28 +17997,36 @@
         <v>2000</v>
       </c>
       <c r="B22">
-        <v>-2.5717400000000001E-2</v>
+        <f>B27-0.0257174</f>
+        <v>0.40609190000000001</v>
       </c>
       <c r="C22">
-        <v>-7.8326699999999985E-2</v>
+        <f>B27-0.0783267</f>
+        <v>0.35348259999999998</v>
       </c>
       <c r="D22">
-        <v>-0.2139875</v>
+        <f>B27-0.2139875</f>
+        <v>0.21782180000000001</v>
       </c>
       <c r="E22">
-        <v>-0.32111109999999998</v>
+        <f>B27-0.3211111</f>
+        <v>0.11069820000000002</v>
       </c>
       <c r="F22">
-        <v>-0.39425060000000001</v>
+        <f>B27-0.3942506</f>
+        <v>3.75587E-2</v>
       </c>
       <c r="G22">
-        <v>-0.42330570000000006</v>
+        <f>B27-0.4233057</f>
+        <v>8.5036E-3</v>
       </c>
       <c r="H22">
-        <v>-0.51994109999999993</v>
+        <f>B27-0.5199411</f>
+        <v>-8.8131800000000038E-2</v>
       </c>
       <c r="I22">
-        <v>-0.54239300000000001</v>
+        <f>B27-0.542393</f>
+        <v>-0.11058370000000001</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -17943,28 +18034,49 @@
         <v>2010</v>
       </c>
       <c r="B23">
-        <v>5.5763800000000002E-2</v>
+        <f>B27+0.0557638</f>
+        <v>0.48757309999999998</v>
       </c>
       <c r="C23">
-        <v>0.187247</v>
+        <f>B27+0.187247</f>
+        <v>0.6190563</v>
       </c>
       <c r="D23">
-        <v>-3.8567699999999996E-2</v>
+        <f>B27-0.0385677</f>
+        <v>0.39324160000000002</v>
       </c>
       <c r="E23">
-        <v>-0.2282469</v>
+        <f>B27-0.2282469</f>
+        <v>0.2035624</v>
       </c>
       <c r="F23">
-        <v>-0.33999800000000002</v>
+        <f>B27-0.339998</f>
+        <v>9.1811299999999985E-2</v>
       </c>
       <c r="G23">
-        <v>-0.42371170000000002</v>
+        <f>B27-0.4237117</f>
+        <v>8.0975999999999826E-3</v>
       </c>
       <c r="H23">
-        <v>-0.51149899999999993</v>
+        <f>B27-0.511499</f>
+        <v>-7.968970000000003E-2</v>
       </c>
       <c r="I23">
-        <v>-0.56449490000000002</v>
+        <f>B27-0.5644949</f>
+        <v>-0.13268560000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27">
+        <v>0.43180930000000001</v>
       </c>
     </row>
   </sheetData>
@@ -19321,10 +19433,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9688483-AFFF-4A20-9820-74818D16B6CF}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19363,22 +19475,28 @@
         <v>237</v>
       </c>
       <c r="B2">
-        <v>-8.2736199999999996E-2</v>
+        <f>B29-0.0827362</f>
+        <v>0.34453690000000003</v>
       </c>
       <c r="C2">
-        <v>-0.1238089</v>
+        <f>B29-0.1238089</f>
+        <v>0.30346420000000002</v>
       </c>
       <c r="D2">
-        <v>-0.10956299999999999</v>
+        <f>B29-0.109563</f>
+        <v>0.3177101</v>
       </c>
       <c r="E2">
-        <v>-1.44046E-2</v>
+        <f>B29-0.0144046</f>
+        <v>0.41286850000000003</v>
       </c>
       <c r="F2">
-        <v>-3.0864900000000001E-2</v>
+        <f>B29-0.0308649</f>
+        <v>0.39640819999999999</v>
       </c>
       <c r="G2">
-        <v>6.1643799999999999E-2</v>
+        <f>B29+0.0616438</f>
+        <v>0.48891689999999999</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -19386,22 +19504,28 @@
         <v>238</v>
       </c>
       <c r="B3">
-        <v>-0.19365070000000001</v>
+        <f>B29-0.1936507</f>
+        <v>0.23362240000000001</v>
       </c>
       <c r="C3">
-        <v>-0.13369059999999999</v>
+        <f>B29-0.1336906</f>
+        <v>0.29358250000000002</v>
       </c>
       <c r="D3">
-        <v>-0.18387580000000001</v>
+        <f>B29-0.1838758</f>
+        <v>0.24339730000000001</v>
       </c>
       <c r="E3">
-        <v>-0.18968409999999999</v>
+        <f>B29-0.1896841</f>
+        <v>0.23758900000000002</v>
       </c>
       <c r="F3">
-        <v>-8.4181500000000006E-2</v>
+        <f>B29-0.0841815</f>
+        <v>0.3430916</v>
       </c>
       <c r="G3">
-        <v>0.1710189</v>
+        <f>B29+0.1710189</f>
+        <v>0.59829200000000005</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -19409,22 +19533,28 @@
         <v>239</v>
       </c>
       <c r="B4">
-        <v>-0.21749609999999997</v>
+        <f>B29-0.2174961</f>
+        <v>0.20977700000000002</v>
       </c>
       <c r="C4">
-        <v>-0.30781799999999998</v>
+        <f>B29-0.307818</f>
+        <v>0.11945510000000004</v>
       </c>
       <c r="D4">
-        <v>-0.362456</v>
+        <f>B29-0.362456</f>
+        <v>6.4817100000000016E-2</v>
       </c>
       <c r="E4">
-        <v>-0.27196239999999999</v>
+        <f>B29-0.2719624</f>
+        <v>0.15531070000000002</v>
       </c>
       <c r="F4">
-        <v>-0.20224349999999999</v>
+        <f>B29-0.2022435</f>
+        <v>0.22502960000000002</v>
       </c>
       <c r="G4">
-        <v>-2.0099500000000006E-2</v>
+        <f>B29-0.0200995</f>
+        <v>0.40717360000000002</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -19432,22 +19562,28 @@
         <v>240</v>
       </c>
       <c r="B5">
-        <v>-0.23572369999999998</v>
+        <f>B29-0.2357237</f>
+        <v>0.19154940000000001</v>
       </c>
       <c r="C5">
-        <v>-0.38977989999999996</v>
+        <f>B29-0.3897799</f>
+        <v>3.7493200000000004E-2</v>
       </c>
       <c r="D5">
-        <v>-0.45770499999999992</v>
+        <f>B29-0.457705</f>
+        <v>-3.0431899999999956E-2</v>
       </c>
       <c r="E5">
-        <v>-0.37527060000000001</v>
+        <f>B29-0.3752706</f>
+        <v>5.2002500000000007E-2</v>
       </c>
       <c r="F5">
-        <v>-0.29594489999999996</v>
+        <f>B29-0.2959449</f>
+        <v>0.13132820000000001</v>
       </c>
       <c r="G5">
-        <v>-0.2021086</v>
+        <f>B29-0.2021086</f>
+        <v>0.22516450000000002</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -19455,22 +19591,28 @@
         <v>241</v>
       </c>
       <c r="B6">
-        <v>-0.41074839999999996</v>
+        <f>B29-0.4107484</f>
+        <v>1.6524700000000003E-2</v>
       </c>
       <c r="C6">
-        <v>-0.49898370000000003</v>
+        <f>B29-0.4989837</f>
+        <v>-7.1710599999999958E-2</v>
       </c>
       <c r="D6">
-        <v>-0.49047819999999998</v>
+        <f>B29-0.4904782</f>
+        <v>-6.3205099999999959E-2</v>
       </c>
       <c r="E6">
-        <v>-0.40029139999999996</v>
+        <f>B29-0.4002914</f>
+        <v>2.6981699999999997E-2</v>
       </c>
       <c r="F6">
-        <v>-0.38855119999999999</v>
+        <f>B29-0.3885512</f>
+        <v>3.8721900000000031E-2</v>
       </c>
       <c r="G6">
-        <v>-0.32179610000000003</v>
+        <f>B29-0.3217961</f>
+        <v>0.10547700000000004</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -19478,22 +19620,28 @@
         <v>242</v>
       </c>
       <c r="B7">
-        <v>-0.54465839999999999</v>
+        <f>B29-0.5446584</f>
+        <v>-0.11738529999999997</v>
       </c>
       <c r="C7">
-        <v>-0.5843453999999999</v>
+        <f>B29-0.5843454</f>
+        <v>-0.1570723</v>
       </c>
       <c r="D7">
-        <v>-0.52644659999999999</v>
+        <f>B29-0.5264466</f>
+        <v>-9.917349999999997E-2</v>
       </c>
       <c r="E7">
-        <v>-0.45588609999999996</v>
+        <f>B29-0.4558861</f>
+        <v>-2.8613E-2</v>
       </c>
       <c r="F7">
-        <v>-0.4227593999999999</v>
+        <f>B29-0.4227594</f>
+        <v>4.5137000000000094E-3</v>
       </c>
       <c r="G7">
-        <v>-0.409551</v>
+        <f>B29-0.409551</f>
+        <v>1.7722100000000018E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -19501,22 +19649,28 @@
         <v>243</v>
       </c>
       <c r="B8">
-        <v>-0.62729639999999998</v>
+        <f>B29-0.6272964</f>
+        <v>-0.20002329999999996</v>
       </c>
       <c r="C8">
-        <v>-0.65378219999999998</v>
+        <f>B29-0.6537822</f>
+        <v>-0.22650909999999996</v>
       </c>
       <c r="D8">
-        <v>-0.60023779999999993</v>
+        <f>B29-0.6002378</f>
+        <v>-0.17296470000000003</v>
       </c>
       <c r="E8">
-        <v>-0.5664518999999999</v>
+        <f>B29-0.5664519</f>
+        <v>-0.13917879999999999</v>
       </c>
       <c r="F8">
-        <v>-0.52368949999999992</v>
+        <f>B29-0.5236895</f>
+        <v>-9.6416400000000013E-2</v>
       </c>
       <c r="G8">
-        <v>-0.50304589999999993</v>
+        <f>B29-0.5030459</f>
+        <v>-7.5772800000000029E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -19524,22 +19678,28 @@
         <v>244</v>
       </c>
       <c r="B9">
-        <v>-0.55715610000000004</v>
+        <f>B29-0.5571561</f>
+        <v>-0.12988300000000003</v>
       </c>
       <c r="C9">
-        <v>-0.61997610000000003</v>
+        <f>B29-0.6199761</f>
+        <v>-0.19270300000000001</v>
       </c>
       <c r="D9">
-        <v>-0.6310135</v>
+        <f>B29-0.6310135</f>
+        <v>-0.20374039999999999</v>
       </c>
       <c r="E9">
-        <v>-0.57389100000000004</v>
+        <f>B29-0.573891</f>
+        <v>-0.14661790000000002</v>
       </c>
       <c r="F9">
-        <v>-0.55308420000000003</v>
+        <f>B29-0.5530842</f>
+        <v>-0.12581110000000001</v>
       </c>
       <c r="G9">
-        <v>-0.56193879999999996</v>
+        <f>B29-0.5619388</f>
+        <v>-0.13466569999999994</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -19584,28 +19744,36 @@
         <v>1960</v>
       </c>
       <c r="B15">
-        <v>-8.2736199999999996E-2</v>
+        <f>B29-0.0827362</f>
+        <v>0.34453690000000003</v>
       </c>
       <c r="C15">
-        <v>-0.19365070000000001</v>
+        <f>B29-0.1936507</f>
+        <v>0.23362240000000001</v>
       </c>
       <c r="D15">
-        <v>-0.21749609999999997</v>
+        <f>B29-0.2174961</f>
+        <v>0.20977700000000002</v>
       </c>
       <c r="E15">
-        <v>-0.23572369999999998</v>
+        <f>B29-0.2357237</f>
+        <v>0.19154940000000001</v>
       </c>
       <c r="F15">
-        <v>-0.41074839999999996</v>
+        <f>B29-0.4107484</f>
+        <v>1.6524700000000003E-2</v>
       </c>
       <c r="G15">
-        <v>-0.54465839999999999</v>
+        <f>B29-0.5446584</f>
+        <v>-0.11738529999999997</v>
       </c>
       <c r="H15">
-        <v>-0.62729639999999998</v>
+        <f>B29-0.6272964</f>
+        <v>-0.20002329999999996</v>
       </c>
       <c r="I15">
-        <v>-0.55715610000000004</v>
+        <f>B29-0.5571561</f>
+        <v>-0.12988300000000003</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -19613,28 +19781,36 @@
         <v>1970</v>
       </c>
       <c r="B16">
-        <v>-0.1238089</v>
+        <f>B29-0.1238089</f>
+        <v>0.30346420000000002</v>
       </c>
       <c r="C16">
-        <v>-0.13369059999999999</v>
+        <f>B29-0.1336906</f>
+        <v>0.29358250000000002</v>
       </c>
       <c r="D16">
-        <v>-0.30781799999999998</v>
+        <f>B29-0.307818</f>
+        <v>0.11945510000000004</v>
       </c>
       <c r="E16">
-        <v>-0.38977989999999996</v>
+        <f>B29-0.3897799</f>
+        <v>3.7493200000000004E-2</v>
       </c>
       <c r="F16">
-        <v>-0.49898370000000003</v>
+        <f>B29-0.4989837</f>
+        <v>-7.1710599999999958E-2</v>
       </c>
       <c r="G16">
-        <v>-0.5843453999999999</v>
+        <f>B29-0.5843454</f>
+        <v>-0.1570723</v>
       </c>
       <c r="H16">
-        <v>-0.65378219999999998</v>
+        <f>B29-0.6537822</f>
+        <v>-0.22650909999999996</v>
       </c>
       <c r="I16">
-        <v>-0.61997610000000003</v>
+        <f>B29-0.6199761</f>
+        <v>-0.19270300000000001</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -19642,28 +19818,36 @@
         <v>1980</v>
       </c>
       <c r="B17">
-        <v>-0.10956299999999999</v>
+        <f>B29-0.109563</f>
+        <v>0.3177101</v>
       </c>
       <c r="C17">
-        <v>-0.18387580000000001</v>
+        <f>B29-0.1838758</f>
+        <v>0.24339730000000001</v>
       </c>
       <c r="D17">
-        <v>-0.362456</v>
+        <f>B29-0.362456</f>
+        <v>6.4817100000000016E-2</v>
       </c>
       <c r="E17">
-        <v>-0.45770499999999992</v>
+        <f>B29-0.457705</f>
+        <v>-3.0431899999999956E-2</v>
       </c>
       <c r="F17">
-        <v>-0.49047819999999998</v>
+        <f>B29-0.4904782</f>
+        <v>-6.3205099999999959E-2</v>
       </c>
       <c r="G17">
-        <v>-0.52644659999999999</v>
+        <f>B29-0.5264466</f>
+        <v>-9.917349999999997E-2</v>
       </c>
       <c r="H17">
-        <v>-0.60023779999999993</v>
+        <f>B29-0.6002378</f>
+        <v>-0.17296470000000003</v>
       </c>
       <c r="I17">
-        <v>-0.6310135</v>
+        <f>B29-0.6310135</f>
+        <v>-0.20374039999999999</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -19671,28 +19855,36 @@
         <v>1990</v>
       </c>
       <c r="B18">
-        <v>-1.44046E-2</v>
+        <f>B29-0.0144046</f>
+        <v>0.41286850000000003</v>
       </c>
       <c r="C18">
-        <v>-0.18968409999999999</v>
+        <f>B29-0.1896841</f>
+        <v>0.23758900000000002</v>
       </c>
       <c r="D18">
-        <v>-0.27196239999999999</v>
+        <f>B29-0.2719624</f>
+        <v>0.15531070000000002</v>
       </c>
       <c r="E18">
-        <v>-0.37527060000000001</v>
+        <f>B29-0.3752706</f>
+        <v>5.2002500000000007E-2</v>
       </c>
       <c r="F18">
-        <v>-0.40029139999999996</v>
+        <f>B29-0.4002914</f>
+        <v>2.6981699999999997E-2</v>
       </c>
       <c r="G18">
-        <v>-0.45588609999999996</v>
+        <f>B29-0.4558861</f>
+        <v>-2.8613E-2</v>
       </c>
       <c r="H18">
-        <v>-0.5664518999999999</v>
+        <f>B29-0.5664519</f>
+        <v>-0.13917879999999999</v>
       </c>
       <c r="I18">
-        <v>-0.57389100000000004</v>
+        <f>B29-0.573891</f>
+        <v>-0.14661790000000002</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -19700,28 +19892,36 @@
         <v>2000</v>
       </c>
       <c r="B19">
-        <v>-3.0864900000000001E-2</v>
+        <f>B29-0.0308649</f>
+        <v>0.39640819999999999</v>
       </c>
       <c r="C19">
-        <v>-8.4181500000000006E-2</v>
+        <f>B29-0.0841815</f>
+        <v>0.3430916</v>
       </c>
       <c r="D19">
-        <v>-0.20224349999999999</v>
+        <f>B29-0.2022435</f>
+        <v>0.22502960000000002</v>
       </c>
       <c r="E19">
-        <v>-0.29594489999999996</v>
+        <f>B29-0.2959449</f>
+        <v>0.13132820000000001</v>
       </c>
       <c r="F19">
-        <v>-0.38855119999999999</v>
+        <f>B29-0.3885512</f>
+        <v>3.8721900000000031E-2</v>
       </c>
       <c r="G19">
-        <v>-0.4227593999999999</v>
+        <f>B29-0.4227594</f>
+        <v>4.5137000000000094E-3</v>
       </c>
       <c r="H19">
-        <v>-0.52368949999999992</v>
+        <f>B29-0.5236895</f>
+        <v>-9.6416400000000013E-2</v>
       </c>
       <c r="I19">
-        <v>-0.55308420000000003</v>
+        <f>B29-0.5530842</f>
+        <v>-0.12581110000000001</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -19729,28 +19929,44 @@
         <v>2010</v>
       </c>
       <c r="B20">
-        <v>6.1643799999999999E-2</v>
+        <f>B29+0.0616438</f>
+        <v>0.48891689999999999</v>
       </c>
       <c r="C20">
-        <v>0.1710189</v>
+        <f>B29+0.1710189</f>
+        <v>0.59829200000000005</v>
       </c>
       <c r="D20">
-        <v>-2.0099500000000006E-2</v>
+        <f>B29-0.0200995</f>
+        <v>0.40717360000000002</v>
       </c>
       <c r="E20">
-        <v>-0.2021086</v>
+        <f>B29-0.2021086</f>
+        <v>0.22516450000000002</v>
       </c>
       <c r="F20">
-        <v>-0.32179610000000003</v>
+        <f>B29-0.3217961</f>
+        <v>0.10547700000000004</v>
       </c>
       <c r="G20">
-        <v>-0.409551</v>
+        <f>B29-0.409551</f>
+        <v>1.7722100000000018E-2</v>
       </c>
       <c r="H20">
-        <v>-0.50304589999999993</v>
+        <f>B29-0.5030459</f>
+        <v>-7.5772800000000029E-2</v>
       </c>
       <c r="I20">
-        <v>-0.56193879999999996</v>
+        <f>B29-0.5619388</f>
+        <v>-0.13466569999999994</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29">
+        <v>0.42727310000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Model With No Lag Vars and Titles to Model with Lag Vars
</commit_message>
<xml_diff>
--- a/output/lnUSDummyModelTripleInteractionlnMortSq2.xlsx
+++ b/output/lnUSDummyModelTripleInteractionlnMortSq2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bz22\Desktop\ComparativeMortality\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA21F60-E2A9-4C01-AD3F-C8CB64E4E9CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DD350E-339C-4388-BD26-026FB3A1438E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3084,6 +3084,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>X Axis is Year Decade; Lines are Age Categories</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4036,6 +4066,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>X Axis is Age Category; Lines are YearDecades</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6593,6 +6653,44 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>X Axis is Year Decade; Lines are Age Categories</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.46883335280335892"/>
+          <c:y val="1.402061582519052E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7545,6 +7643,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>X Axis is Age Category; Lines are YearDecades</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12899,16 +13027,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>138111</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>61911</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12935,16 +13063,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2043112</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>42861</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>319087</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>90486</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13053,16 +13181,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>638735</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>33617</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1804147</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>112058</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>481852</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>134471</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>112057</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13089,16 +13217,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>431425</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>34737</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1428749</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>135590</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>403412</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>100852</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1400736</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>11205</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16033,12 +16161,12 @@
   <dimension ref="A1:AA50"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -17543,8 +17671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6752113A-E80F-4D8E-962A-42C6198FCF3D}">
   <dimension ref="A2:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="J10" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Resize Axes on tripleinteraction model lnmortsq2
</commit_message>
<xml_diff>
--- a/output/lnUSDummyModelTripleInteractionlnMortSq2.xlsx
+++ b/output/lnUSDummyModelTripleInteractionlnMortSq2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bz22\Desktop\ComparativeMortality\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DD350E-339C-4388-BD26-026FB3A1438E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0E6B85-8870-4935-A29A-17AB071DE628}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6687,8 +6687,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.46883335280335892"/>
-          <c:y val="1.402061582519052E-2"/>
+          <c:x val="0.3366299512104588"/>
+          <c:y val="1.8694154433587361E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -7493,6 +7493,8 @@
         <c:axId val="1388557408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="-0.60000000000000009"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -8363,6 +8365,8 @@
         <c:axId val="1391878656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="-0.60000000000000009"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -13182,15 +13186,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1804147</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>112058</xdr:rowOff>
+      <xdr:colOff>470647</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>112057</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>22412</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>593910</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>89648</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13218,15 +13222,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1428749</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>135590</xdr:rowOff>
+      <xdr:colOff>296956</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>23531</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1400736</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>11205</xdr:rowOff>
+      <xdr:colOff>268943</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>89646</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>

<commit_message>
Added Triple Interactions Memo
</commit_message>
<xml_diff>
--- a/output/lnUSDummyModelTripleInteractionlnMortSq2.xlsx
+++ b/output/lnUSDummyModelTripleInteractionlnMortSq2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bz22\Desktop\ComparativeMortality\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0E6B85-8870-4935-A29A-17AB071DE628}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D2DA4D-1CB5-4E51-BFC0-41E438932622}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lnUSDummyModelTripleInteraction" sheetId="1" r:id="rId1"/>
@@ -12990,16 +12990,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>208250</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>330714</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>169408</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>47</xdr:col>
-      <xdr:colOff>327314</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>449778</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>88446</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13557,7 +13557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C237"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:C19"/>
     </sheetView>
   </sheetViews>
@@ -16164,8 +16164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19567,7 +19567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9688483-AFFF-4A20-9820-74818D16B6CF}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>

</xml_diff>